<commit_message>
Ran scenarios 100 times and created mean and std of results
</commit_message>
<xml_diff>
--- a/Scenario pasient-data.xlsx
+++ b/Scenario pasient-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\There\PycharmProjects\ABM---hospital\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC67AC35-06BF-4557-A666-2F42838A90CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D7D928-9FE3-4BFB-8F14-54E6FB3B34B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{3D08B538-DB8C-4D4E-BD62-B68A7ED57B49}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3D08B538-DB8C-4D4E-BD62-B68A7ED57B49}"/>
   </bookViews>
   <sheets>
     <sheet name="Prediksjon sykdomstall" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Populasjon</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>AHUS-innlagte-r 1.1 scenario lav</t>
+  </si>
+  <si>
+    <t>Sum pasienter 60 dager</t>
+  </si>
+  <si>
+    <t>Sum smittede</t>
   </si>
 </sst>
 </file>
@@ -471,8 +477,8 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:T112"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D112"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
@@ -1598,6 +1604,12 @@
         <f t="shared" si="7"/>
         <v>25.191632656601275</v>
       </c>
+      <c r="M22" t="s">
+        <v>28</v>
+      </c>
+      <c r="P22" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1643,9 +1655,25 @@
         <f t="shared" si="7"/>
         <v>24.831752190078397</v>
       </c>
+      <c r="M23">
+        <f>SUM(B2:B62)</f>
+        <v>1024682.6789310077</v>
+      </c>
       <c r="N23">
-        <f>SUM(F3:F62)</f>
-        <v>837.05188502609849</v>
+        <f>M23*0.109</f>
+        <v>111690.41200347984</v>
+      </c>
+      <c r="O23">
+        <f>N23*0.0012</f>
+        <v>134.0284944041758</v>
+      </c>
+      <c r="P23">
+        <f>SUM(F2:F62)</f>
+        <v>837.67809002609852</v>
+      </c>
+      <c r="Q23">
+        <f>P23*0.029</f>
+        <v>24.292664610756859</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -1692,9 +1720,25 @@
         <f t="shared" si="7"/>
         <v>24.477012873077282</v>
       </c>
+      <c r="M24">
+        <f>SUM(G2:G62)</f>
+        <v>841281.35577732231</v>
+      </c>
       <c r="N24">
-        <f>SUM(K3:K62)</f>
-        <v>916.16173779728115</v>
+        <f>M24*0.109</f>
+        <v>91699.66777972813</v>
+      </c>
+      <c r="O24">
+        <f>N24*0.0012</f>
+        <v>110.03960133567375</v>
+      </c>
+      <c r="P24">
+        <f>SUM(K2:K62)</f>
+        <v>916.99667779728111</v>
+      </c>
+      <c r="Q24">
+        <f>P24*0.029</f>
+        <v>26.592903656121152</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -5671,10 +5715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7D5BB8-8042-41E8-B2B8-6F2B060ED930}">
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E112"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
@@ -6289,7 +6333,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43931</v>
       </c>
@@ -6308,7 +6352,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43932</v>
       </c>
@@ -6327,7 +6371,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43933</v>
       </c>
@@ -6346,7 +6390,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43934</v>
       </c>
@@ -6365,7 +6409,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43935</v>
       </c>
@@ -6383,8 +6427,12 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <f>_xlfn.DAYS(A38,A2)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43936</v>
       </c>
@@ -6403,7 +6451,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43937</v>
       </c>
@@ -6422,7 +6470,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43938</v>
       </c>
@@ -6441,7 +6489,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43939</v>
       </c>
@@ -6460,7 +6508,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43940</v>
       </c>
@@ -6479,7 +6527,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43941</v>
       </c>
@@ -6498,7 +6546,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43942</v>
       </c>
@@ -6517,7 +6565,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43943</v>
       </c>
@@ -6536,7 +6584,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43944</v>
       </c>
@@ -6555,7 +6603,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43945</v>
       </c>
@@ -6574,7 +6622,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43946</v>
       </c>

</xml_diff>